<commit_message>
Sesión 7 y proyectos alumnos
</commit_message>
<xml_diff>
--- a/proyectos/Proyecto alumnos.xlsx
+++ b/proyectos/Proyecto alumnos.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/IPN-DEEP_LEARNING/diplomado/proyectos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB93268-F296-CB43-9FE1-66AFA037712B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3072FDD-BE3C-0B47-A161-B0E755D04853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37560" yWindow="-2540" windowWidth="27640" windowHeight="15800" activeTab="1" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="138">
   <si>
     <r>
       <t>Instructor:</t>
@@ -466,6 +467,59 @@
     <t>* Ruta aprendizaje
 * Técnicas de estudio
 * Tabla de itinerario semanal con 4 puntos de aprendizaje por sesión (duración, tema, pre-requisitos)</t>
+  </si>
+  <si>
+    <t>Reconocimiento de firmas y sellos en documentos</t>
+  </si>
+  <si>
+    <t>Solicitar la imagen del documento</t>
+  </si>
+  <si>
+    <t>* Lista de comprobaciones si se contienen nombres, firmas y sellos
+* Extraer las coordenadas o la subimagen del sello
+* Generar una clasificación entre distintos tipos de sellos</t>
+  </si>
+  <si>
+    <t>Contador de calorías</t>
+  </si>
+  <si>
+    <t>Solicitar la imagen del platillo o empaque</t>
+  </si>
+  <si>
+    <t>* Listar los ingredientes
+* Tabla con gramajes
+* Aumentar las calorías por unidad</t>
+  </si>
+  <si>
+    <t>Extracción de caducidad</t>
+  </si>
+  <si>
+    <t>Solicitar la imagen del producto en la zona de caducidad (escaneo)</t>
+  </si>
+  <si>
+    <t>* Lista de textos que reconoces
+* Lista con fechas específicas
+* Aumentar los días positivos o negativos de caducidad</t>
+  </si>
+  <si>
+    <t>Analizador de resultados clínicos</t>
+  </si>
+  <si>
+    <t>Solicitar los resultados clínicos del análisis de sangre u otros</t>
+  </si>
+  <si>
+    <t>* Texto simplificado de los resultados
+* Valores de referencia explicados acorde a los resultados
+* Lista de recomendaciones sin incluir medicamentos, únicamente ejercicios y dieta</t>
+  </si>
+  <si>
+    <t>ENTREGADO</t>
+  </si>
+  <si>
+    <t>PRESENTADO</t>
+  </si>
+  <si>
+    <t>CORREO</t>
   </si>
 </sst>
 </file>
@@ -557,7 +611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +628,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1007,11 +1073,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1019,7 +1084,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1031,87 +1095,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1120,9 +1106,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1190,6 +1173,110 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,64 +1427,124 @@
     </xdr:sp>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>101600</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>685800</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBCFF618-B64B-E248-8D0D-1BCEE518D774}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s1025"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBCFF618-B64B-E248-8D0D-1BCEE518D774}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="TextBox1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E8CAF6-A44E-46E0-94D9-FCA947A5B69F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8356600" y="152400"/>
+          <a:ext cx="3060700" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1717,7 +1864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9C8F5D-2E50-B94A-A968-16D5A925CB44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9C8F5D-2E50-B94A-A968-16D5A925CB44}">
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1727,819 +1874,819 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19" t="s">
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21" t="s">
+      <c r="K4" s="39"/>
+      <c r="L4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="20"/>
+      <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="30"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="41"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="38"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="16">
         <v>3</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="16">
         <v>4</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="16">
         <v>6</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="16">
         <v>10</v>
       </c>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="45" t="s">
+      <c r="L8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="46">
+      <c r="A9" s="17">
         <v>1</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
+      <c r="A10" s="23">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
+      <c r="A11" s="23">
         <v>3</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="46">
+      <c r="A12" s="17">
         <v>4</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="46">
+      <c r="A13" s="17">
         <v>5</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
+      <c r="A14" s="23">
         <v>6</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+      <c r="A15" s="23">
         <v>7</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="46">
+      <c r="A16" s="17">
         <v>8</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="46">
+      <c r="A17" s="17">
         <v>9</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="52">
+      <c r="A18" s="23">
         <v>10</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="52">
+      <c r="A19" s="23">
         <v>11</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="53"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="46">
+      <c r="A20" s="17">
         <v>12</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="49" t="s">
+      <c r="D20" s="26"/>
+      <c r="E20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="46">
+      <c r="A21" s="17">
         <v>13</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="53"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="52">
+      <c r="A22" s="23">
         <v>14</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="52">
+      <c r="A23" s="23">
         <v>15</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="53"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="46">
+      <c r="A24" s="17">
         <v>16</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="46">
+      <c r="A25" s="17">
         <v>17</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="53"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="52">
+      <c r="A26" s="23">
         <v>18</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="49" t="s">
+      <c r="D26" s="26"/>
+      <c r="E26" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="52">
+      <c r="A27" s="23">
         <v>19</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="46">
+      <c r="A28" s="17">
         <v>20</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="46">
+      <c r="A29" s="17">
         <v>21</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="53"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="52">
+      <c r="A30" s="23">
         <v>22</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="57"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="52">
+      <c r="A31" s="23">
         <v>23</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49" t="s">
+      <c r="D31" s="20"/>
+      <c r="E31" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="46">
+      <c r="A32" s="17">
         <v>24</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="49" t="s">
+      <c r="D32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="53"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="46">
+      <c r="A33" s="17">
         <v>25</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49" t="s">
+      <c r="D33" s="20"/>
+      <c r="E33" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="52">
+      <c r="A34" s="23">
         <v>26</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49" t="s">
+      <c r="D34" s="20"/>
+      <c r="E34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="54"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
+      <c r="A35" s="23">
         <v>27</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="53"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="58"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60">
+      <c r="A36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31">
         <v>14</v>
       </c>
-      <c r="E36" s="61">
+      <c r="E36" s="32">
         <v>13</v>
       </c>
-      <c r="J36" s="62"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="63"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2552,8 +2699,8 @@
     <mergeCell ref="J4:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2584,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114E1FA5-8B4D-4C49-884E-96E44BB25D99}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A24" zoomScale="82" workbookViewId="0">
+      <selection activeCell="B28" sqref="A1:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2596,13 +2743,14 @@
     <col min="3" max="3" width="55.33203125" customWidth="1"/>
     <col min="4" max="4" width="66.33203125" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
@@ -2615,19 +2763,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="46">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="67">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="52">
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="18" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
@@ -2636,15 +2784,15 @@
       <c r="D3" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="52">
+    <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="71">
         <v>3</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C4" t="s">
@@ -2653,23 +2801,26 @@
       <c r="D4" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="37" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="46">
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="67">
         <v>4</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="68" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="46">
+    <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="70">
         <v>5</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C6" t="s">
@@ -2678,15 +2829,21 @@
       <c r="D6" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
+      <c r="F6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="71">
         <v>6</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C7" t="s">
@@ -2695,23 +2852,26 @@
       <c r="D7" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="37" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="52">
+      <c r="F7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="69">
         <v>7</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="68" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="46">
+    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="70">
         <v>8</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
@@ -2720,31 +2880,43 @@
       <c r="D9" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="37" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="46">
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="67">
         <v>9</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="68" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="18" t="s">
         <v>42</v>
       </c>
       <c r="C12" t="s">
@@ -2757,27 +2929,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="46">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="67">
         <v>12</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="46">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="67">
         <v>13</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="68" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+    <row r="15" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="71">
         <v>14</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C15" t="s">
@@ -2786,47 +2958,83 @@
       <c r="D15" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="37" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="52">
+      <c r="F15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" s="71">
         <v>15</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="46">
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="70">
         <v>16</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="46">
+      <c r="C17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="52">
+      <c r="C18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="69">
         <v>18</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="68" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="52">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="71">
         <v>19</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C20" t="s">
@@ -2838,12 +3046,15 @@
       <c r="E20" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="46">
+      <c r="F20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="70">
         <v>20</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="18" t="s">
         <v>60</v>
       </c>
       <c r="C21" t="s">
@@ -2852,15 +3063,18 @@
       <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="37" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="46">
+      <c r="F21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="70">
         <v>21</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C22" t="s">
@@ -2872,12 +3086,15 @@
       <c r="E22" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="153" x14ac:dyDescent="0.2">
-      <c r="A23" s="52">
+      <c r="F22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A23" s="71">
         <v>22</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="18" t="s">
         <v>64</v>
       </c>
       <c r="C23" t="s">
@@ -2886,15 +3103,18 @@
       <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A24" s="52">
+      <c r="F23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" s="71">
         <v>23</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="18" t="s">
         <v>66</v>
       </c>
       <c r="C24" t="s">
@@ -2903,15 +3123,18 @@
       <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="37" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="46">
+      <c r="F24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="72">
         <v>24</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="18" t="s">
         <v>68</v>
       </c>
       <c r="C25" t="s">
@@ -2920,15 +3143,15 @@
       <c r="D25" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="46">
+    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="70">
         <v>25</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
       <c r="C26" t="s">
@@ -2937,23 +3160,272 @@
       <c r="D26" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="66" t="s">
+      <c r="E26" s="37" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="52">
+      <c r="F26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="69">
         <v>26</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="52">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="71">
         <v>27</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692E3E0D-50B9-9E4B-8DA7-9E1A64156276}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="A1:B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="67">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="71">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="67">
+        <v>4</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="70">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="71">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="69">
+        <v>7</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="70">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="67">
+        <v>9</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="67">
+        <v>12</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="67">
+        <v>13</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="71">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="71">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="70">
+        <v>16</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="69">
+        <v>18</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="71">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="70">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="70">
+        <v>21</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="71">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="71">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="72">
+        <v>24</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="70">
+        <v>25</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="69">
+        <v>26</v>
+      </c>
+      <c r="B27" s="68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="71">
+        <v>27</v>
+      </c>
+      <c r="B28" s="73" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sesión 10 y proyectos alumnos
</commit_message>
<xml_diff>
--- a/proyectos/Proyecto alumnos.xlsx
+++ b/proyectos/Proyecto alumnos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/IPN-DEEP_LEARNING/diplomado/proyectos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3072FDD-BE3C-0B47-A161-B0E755D04853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF3262F-643D-CC4B-A063-A9539EEF1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
   <si>
     <r>
       <t>Instructor:</t>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>CORREO</t>
+  </si>
+  <si>
+    <t>•</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,6 +642,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1174,6 +1195,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1257,26 +1293,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1874,10 +1904,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1925,29 +1955,29 @@
         <v>4</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="64" t="s">
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="38" t="s">
+      <c r="K4" s="44"/>
+      <c r="L4" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="39"/>
+      <c r="M4" s="44"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1956,37 +1986,37 @@
       <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="41"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="46"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="43"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="47"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -2005,7 +2035,7 @@
       <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
@@ -2733,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114E1FA5-8B4D-4C49-884E-96E44BB25D99}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B28" sqref="A1:B28"/>
+    <sheetView topLeftCell="D22" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F26" sqref="F3:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2764,10 +2794,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="67">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="39" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2789,7 +2819,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="71">
+      <c r="A4" s="42">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -2809,15 +2839,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="67">
+      <c r="A5" s="38">
         <v>4</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="39" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="70">
+      <c r="A6" s="41">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -2840,7 +2870,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="71">
+      <c r="A7" s="42">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -2860,15 +2890,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="69">
+      <c r="A8" s="40">
         <v>7</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="39" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="70">
+      <c r="A9" s="41">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -2888,10 +2918,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="67">
+      <c r="A10" s="38">
         <v>9</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="39" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2930,23 +2960,23 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="67">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="67">
+      <c r="A14" s="38">
         <v>13</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="39" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="71">
+      <c r="A15" s="42">
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
@@ -2966,7 +2996,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="71">
+      <c r="A16" s="42">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -2986,7 +3016,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="70">
+      <c r="A17" s="41">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -3023,15 +3053,15 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="69">
+      <c r="A19" s="40">
         <v>18</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="71">
+      <c r="A20" s="42">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -3051,7 +3081,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="70">
+      <c r="A21" s="41">
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
@@ -3071,7 +3101,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="70">
+      <c r="A22" s="41">
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
@@ -3091,7 +3121,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="153" x14ac:dyDescent="0.2">
-      <c r="A23" s="71">
+      <c r="A23" s="42">
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -3111,7 +3141,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A24" s="71">
+      <c r="A24" s="42">
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -3131,7 +3161,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="72">
+      <c r="A25" s="17">
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -3148,7 +3178,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="70">
+      <c r="A26" s="41">
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3168,18 +3198,18 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="69">
+      <c r="A27" s="40">
         <v>26</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="39" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="71">
+      <c r="A28" s="42">
         <v>27</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C28" t="s">
@@ -3194,34 +3224,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692E3E0D-50B9-9E4B-8DA7-9E1A64156276}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="A1:B28"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="67">
+      <c r="C1" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -3229,71 +3267,89 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="71">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="42">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="67">
+      <c r="C4" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
         <v>4</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="70">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="74">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="71">
+      <c r="C6" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="42">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="69">
+      <c r="C7" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="40">
         <v>7</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="70">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="67">
+      <c r="C9" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="38">
         <v>9</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="23">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="42">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -3301,47 +3357,59 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="67">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="67">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="38">
         <v>13</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="71">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="42">
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="71">
+      <c r="C15" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="42">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="70">
+      <c r="C16" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="74">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -3349,84 +3417,117 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="69">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="75">
         <v>18</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="72" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="71">
+      <c r="C19" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="42">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="70">
+      <c r="C20" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="41">
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="70">
+      <c r="C21" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="41">
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="71">
+      <c r="C22" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="42">
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="71">
+      <c r="C23" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="42">
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="72">
+      <c r="C24" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="76">
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="70">
+      <c r="C25" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="41">
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="69">
+      <c r="C26" s="73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="40">
         <v>26</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="39" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="71">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="42">
         <v>27</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="18" t="s">
         <v>74</v>
+      </c>
+      <c r="C28" s="73" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sesión 11 y entrega de proyectos
</commit_message>
<xml_diff>
--- a/proyectos/Proyecto alumnos.xlsx
+++ b/proyectos/Proyecto alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/IPN-DEEP_LEARNING/diplomado/proyectos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF3262F-643D-CC4B-A063-A9539EEF1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86E81DE-DD93-634A-8730-860979CA5480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
+    <workbookView xWindow="-36020" yWindow="-2960" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{65B320A6-E656-C34A-A2F8-F5BA0089AEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="139">
   <si>
     <r>
       <t>Instructor:</t>
@@ -614,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,12 +654,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,6 +1204,18 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,19 +1299,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1904,10 +1898,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="54"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1955,29 +1949,29 @@
         <v>4</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="69" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="43" t="s">
+      <c r="K4" s="48"/>
+      <c r="L4" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="44"/>
+      <c r="M4" s="48"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1986,37 +1980,37 @@
       <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="48"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="52"/>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="52"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -2035,7 +2029,7 @@
       <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="53"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
@@ -3227,14 +3221,14 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="73" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="73"/>
+    <col min="3" max="3" width="12.1640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3244,10 +3238,10 @@
       <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="44" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3268,13 +3262,16 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="42">
+      <c r="A4" s="46">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3287,27 +3284,30 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="74">
+      <c r="A6" s="45">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="42">
+      <c r="A7" s="46">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3320,13 +3320,16 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="41">
+      <c r="A9" s="45">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3339,13 +3342,16 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="42">
+      <c r="A11" s="46">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3358,10 +3364,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="38">
+      <c r="A13" s="76">
         <v>12</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="43" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3374,38 +3380,44 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="42">
+      <c r="A15" s="46">
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D15" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="42">
+      <c r="A16" s="46">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D16" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="74">
+      <c r="A17" s="45">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3418,96 +3430,114 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="75">
+      <c r="A19" s="46">
         <v>18</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="42">
+      <c r="A20" s="46">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D20" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="41">
+      <c r="A21" s="45">
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D21" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="41">
+      <c r="A22" s="45">
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D22" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="42">
+      <c r="A23" s="46">
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D23" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="42">
+      <c r="A24" s="46">
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="44" t="s">
         <v>138</v>
       </c>
+      <c r="D24" s="44" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="76">
+      <c r="A25" s="45">
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="73" t="s">
+      <c r="D25" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="41">
+      <c r="A26" s="45">
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="C26" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="44" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3520,13 +3550,16 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="42">
+      <c r="A28" s="46">
         <v>27</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="44" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>